<commit_message>
add pre_dist to each activity as a random number
</commit_message>
<xml_diff>
--- a/template/activity_table.xlsx
+++ b/template/activity_table.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20379"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\cns\navi-master\navi\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\DOCUME~1\MobaXterm\slash\RemoteFiles\722556_4_11\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486AE113-6983-4C77-A21C-EF13CA4FEBFA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11980" windowHeight="9550"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11976" windowHeight="9552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="activity_list" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="414">
   <si>
     <t>code</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -1266,12 +1267,16 @@
   </si>
   <si>
     <t>D12020</t>
+  </si>
+  <si>
+    <t>pre_dist</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2182,23 +2187,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E172"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="16.9140625" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="28.1640625" customWidth="1"/>
-    <col min="4" max="4" width="12.9140625" customWidth="1"/>
-    <col min="1999" max="2000" width="2.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.8984375" customWidth="1"/>
+    <col min="2" max="2" width="20.69921875" customWidth="1"/>
+    <col min="3" max="3" width="28.19921875" customWidth="1"/>
+    <col min="4" max="4" width="12.8984375" customWidth="1"/>
+    <col min="1999" max="2000" width="2.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>230</v>
       </c>
@@ -2214,8 +2219,11 @@
       <c r="E1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -2231,8 +2239,12 @@
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F2">
+        <f ca="1">RANDBETWEEN(0,10)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -2248,8 +2260,12 @@
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F3">
+        <f t="shared" ref="F3:F66" ca="1" si="0">RANDBETWEEN(0,10)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2265,8 +2281,12 @@
       <c r="E4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2282,8 +2302,12 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2299,8 +2323,12 @@
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2316,8 +2344,12 @@
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2333,8 +2365,12 @@
       <c r="E8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2350,8 +2386,12 @@
       <c r="E9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2367,8 +2407,12 @@
       <c r="E10">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2384,8 +2428,12 @@
       <c r="E11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2401,8 +2449,12 @@
       <c r="E12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2418,8 +2470,12 @@
       <c r="E13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2435,8 +2491,12 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2452,8 +2512,12 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2469,8 +2533,12 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2486,8 +2554,12 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2503,8 +2575,12 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2520,8 +2596,12 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F19">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2537,8 +2617,12 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F20">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2554,8 +2638,12 @@
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F21">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2571,8 +2659,12 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F22">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -2588,8 +2680,12 @@
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F23">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -2605,8 +2701,12 @@
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F24">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -2622,8 +2722,12 @@
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F25">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -2639,8 +2743,12 @@
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F26">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -2656,8 +2764,12 @@
       <c r="E27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F27">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -2673,8 +2785,12 @@
       <c r="E28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F28">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -2690,8 +2806,12 @@
       <c r="E29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F29">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -2707,8 +2827,12 @@
       <c r="E30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F30">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -2724,8 +2848,12 @@
       <c r="E31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F31">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -2741,8 +2869,12 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F32">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -2758,8 +2890,12 @@
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F33">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -2775,8 +2911,12 @@
       <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F34">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -2792,8 +2932,12 @@
       <c r="E35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F35">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -2809,8 +2953,12 @@
       <c r="E36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F36">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -2826,8 +2974,12 @@
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F37">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -2843,8 +2995,12 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F38">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -2860,8 +3016,12 @@
       <c r="E39">
         <v>10</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F39">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -2877,8 +3037,12 @@
       <c r="E40">
         <v>5</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F40">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A41" t="s">
         <v>50</v>
       </c>
@@ -2894,8 +3058,12 @@
       <c r="E41">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F41">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -2911,8 +3079,12 @@
       <c r="E42">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F42">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A43" t="s">
         <v>50</v>
       </c>
@@ -2928,8 +3100,12 @@
       <c r="E43">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F43">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>50</v>
       </c>
@@ -2945,8 +3121,12 @@
       <c r="E44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F44">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A45" t="s">
         <v>50</v>
       </c>
@@ -2962,8 +3142,12 @@
       <c r="E45">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F45">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -2979,8 +3163,12 @@
       <c r="E46">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F46">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A47" t="s">
         <v>50</v>
       </c>
@@ -2996,8 +3184,12 @@
       <c r="E47">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F47">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A48" t="s">
         <v>50</v>
       </c>
@@ -3013,8 +3205,12 @@
       <c r="E48">
         <v>10</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F48">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -3030,8 +3226,12 @@
       <c r="E49">
         <v>10</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F49">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3047,8 +3247,12 @@
       <c r="E50">
         <v>10</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F50">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -3064,8 +3268,12 @@
       <c r="E51">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F51">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -3081,8 +3289,12 @@
       <c r="E52">
         <v>5</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F52">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -3098,8 +3310,12 @@
       <c r="E53">
         <v>10</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F53">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A54" t="s">
         <v>64</v>
       </c>
@@ -3115,8 +3331,12 @@
       <c r="E54">
         <v>10</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F54">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A55" t="s">
         <v>64</v>
       </c>
@@ -3132,8 +3352,12 @@
       <c r="E55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F55">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -3149,8 +3373,12 @@
       <c r="E56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F56">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>64</v>
       </c>
@@ -3166,8 +3394,12 @@
       <c r="E57">
         <v>5</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F57">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>70</v>
       </c>
@@ -3183,8 +3415,12 @@
       <c r="E58">
         <v>10</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F58">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>70</v>
       </c>
@@ -3200,8 +3436,12 @@
       <c r="E59">
         <v>3</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F59">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>70</v>
       </c>
@@ -3217,8 +3457,12 @@
       <c r="E60">
         <v>3</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F60">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>70</v>
       </c>
@@ -3234,8 +3478,12 @@
       <c r="E61">
         <v>3</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F61">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -3251,8 +3499,12 @@
       <c r="E62">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F62">
+        <f t="shared" ca="1" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>70</v>
       </c>
@@ -3268,8 +3520,12 @@
       <c r="E63">
         <v>5</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F63">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>70</v>
       </c>
@@ -3285,8 +3541,12 @@
       <c r="E64">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F64">
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>81</v>
       </c>
@@ -3302,8 +3562,12 @@
       <c r="E65">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F65">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>81</v>
       </c>
@@ -3319,8 +3583,12 @@
       <c r="E66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F66">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>81</v>
       </c>
@@ -3336,8 +3604,12 @@
       <c r="E67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F67">
+        <f t="shared" ref="F67:F130" ca="1" si="1">RANDBETWEEN(0,10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>81</v>
       </c>
@@ -3353,8 +3625,12 @@
       <c r="E68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F68">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>81</v>
       </c>
@@ -3370,8 +3646,12 @@
       <c r="E69">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F69">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>81</v>
       </c>
@@ -3387,8 +3667,12 @@
       <c r="E70">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F70">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>81</v>
       </c>
@@ -3404,8 +3688,12 @@
       <c r="E71">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F71">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -3421,8 +3709,12 @@
       <c r="E72">
         <v>5</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F72">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>90</v>
       </c>
@@ -3438,8 +3730,12 @@
       <c r="E73">
         <v>5</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F73">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A74" t="s">
         <v>90</v>
       </c>
@@ -3455,8 +3751,12 @@
       <c r="E74">
         <v>3</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F74">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A75" t="s">
         <v>90</v>
       </c>
@@ -3472,8 +3772,12 @@
       <c r="E75">
         <v>3</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F75">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A76" t="s">
         <v>90</v>
       </c>
@@ -3489,8 +3793,12 @@
       <c r="E76">
         <v>3</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F76">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A77" t="s">
         <v>90</v>
       </c>
@@ -3506,8 +3814,12 @@
       <c r="E77">
         <v>5</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F77">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A78" t="s">
         <v>90</v>
       </c>
@@ -3523,8 +3835,12 @@
       <c r="E78">
         <v>5</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F78">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A79" t="s">
         <v>90</v>
       </c>
@@ -3540,8 +3856,12 @@
       <c r="E79">
         <v>5</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F79">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A80" t="s">
         <v>90</v>
       </c>
@@ -3557,8 +3877,12 @@
       <c r="E80">
         <v>3</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F80">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A81" t="s">
         <v>90</v>
       </c>
@@ -3574,8 +3898,12 @@
       <c r="E81">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F81">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A82" t="s">
         <v>90</v>
       </c>
@@ -3591,8 +3919,12 @@
       <c r="E82">
         <v>3</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F82">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A83" t="s">
         <v>90</v>
       </c>
@@ -3608,8 +3940,12 @@
       <c r="E83">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F83">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A84" t="s">
         <v>90</v>
       </c>
@@ -3625,8 +3961,12 @@
       <c r="E84">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F84">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -3642,8 +3982,12 @@
       <c r="E85">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F85">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>90</v>
       </c>
@@ -3659,8 +4003,12 @@
       <c r="E86">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F86">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>90</v>
       </c>
@@ -3676,8 +4024,12 @@
       <c r="E87">
         <v>3</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F87">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>108</v>
       </c>
@@ -3693,8 +4045,12 @@
       <c r="E88">
         <v>2</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F88">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>108</v>
       </c>
@@ -3710,8 +4066,12 @@
       <c r="E89">
         <v>2</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F89">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>108</v>
       </c>
@@ -3727,8 +4087,12 @@
       <c r="E90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F90">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>108</v>
       </c>
@@ -3744,8 +4108,12 @@
       <c r="E91">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F91">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>108</v>
       </c>
@@ -3761,8 +4129,12 @@
       <c r="E92">
         <v>2</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F92">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>108</v>
       </c>
@@ -3778,8 +4150,12 @@
       <c r="E93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F93">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A94" t="s">
         <v>108</v>
       </c>
@@ -3795,8 +4171,12 @@
       <c r="E94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F94">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A95" t="s">
         <v>108</v>
       </c>
@@ -3812,8 +4192,12 @@
       <c r="E95">
         <v>2</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F95">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A96" t="s">
         <v>108</v>
       </c>
@@ -3829,8 +4213,12 @@
       <c r="E96">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F96">
+        <f t="shared" ca="1" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A97" t="s">
         <v>108</v>
       </c>
@@ -3846,8 +4234,12 @@
       <c r="E97">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F97">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>123</v>
       </c>
@@ -3863,8 +4255,12 @@
       <c r="E98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F98">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>123</v>
       </c>
@@ -3880,8 +4276,12 @@
       <c r="E99">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F99">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>123</v>
       </c>
@@ -3897,8 +4297,12 @@
       <c r="E100">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F100">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A101" t="s">
         <v>123</v>
       </c>
@@ -3914,8 +4318,12 @@
       <c r="E101">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F101">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A102" t="s">
         <v>123</v>
       </c>
@@ -3931,8 +4339,12 @@
       <c r="E102">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F102">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A103" t="s">
         <v>123</v>
       </c>
@@ -3948,8 +4360,12 @@
       <c r="E103">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F103">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A104" t="s">
         <v>123</v>
       </c>
@@ -3965,8 +4381,12 @@
       <c r="E104">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F104">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A105" t="s">
         <v>123</v>
       </c>
@@ -3982,8 +4402,12 @@
       <c r="E105">
         <v>2</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F105">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A106" t="s">
         <v>123</v>
       </c>
@@ -3999,8 +4423,12 @@
       <c r="E106">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F106">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A107" t="s">
         <v>123</v>
       </c>
@@ -4016,8 +4444,12 @@
       <c r="E107">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F107">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A108" t="s">
         <v>123</v>
       </c>
@@ -4033,8 +4465,12 @@
       <c r="E108">
         <v>1</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F108">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A109" t="s">
         <v>123</v>
       </c>
@@ -4050,8 +4486,12 @@
       <c r="E109">
         <v>1</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F109">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A110" t="s">
         <v>123</v>
       </c>
@@ -4067,8 +4507,12 @@
       <c r="E110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F110">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A111" t="s">
         <v>123</v>
       </c>
@@ -4084,8 +4528,12 @@
       <c r="E111">
         <v>1</v>
       </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F111">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A112" t="s">
         <v>123</v>
       </c>
@@ -4101,8 +4549,12 @@
       <c r="E112">
         <v>1</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F112">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A113" t="s">
         <v>123</v>
       </c>
@@ -4118,8 +4570,12 @@
       <c r="E113">
         <v>1</v>
       </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F113">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A114" t="s">
         <v>123</v>
       </c>
@@ -4135,8 +4591,12 @@
       <c r="E114">
         <v>1</v>
       </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F114">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A115" t="s">
         <v>123</v>
       </c>
@@ -4152,8 +4612,12 @@
       <c r="E115">
         <v>1</v>
       </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F115">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A116" t="s">
         <v>123</v>
       </c>
@@ -4169,8 +4633,12 @@
       <c r="E116">
         <v>1</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F116">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -4186,8 +4654,12 @@
       <c r="E117">
         <v>1</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F117">
+        <f t="shared" ca="1" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A118" t="s">
         <v>123</v>
       </c>
@@ -4203,8 +4675,12 @@
       <c r="E118">
         <v>2</v>
       </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F118">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A119" t="s">
         <v>123</v>
       </c>
@@ -4220,8 +4696,12 @@
       <c r="E119">
         <v>1</v>
       </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F119">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A120" t="s">
         <v>123</v>
       </c>
@@ -4237,8 +4717,12 @@
       <c r="E120">
         <v>1</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F120">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A121" t="s">
         <v>123</v>
       </c>
@@ -4254,8 +4738,12 @@
       <c r="E121">
         <v>1</v>
       </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F121">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A122" t="s">
         <v>123</v>
       </c>
@@ -4271,8 +4759,12 @@
       <c r="E122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F122">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -4288,8 +4780,12 @@
       <c r="E123">
         <v>1</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F123">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -4305,8 +4801,12 @@
       <c r="E124">
         <v>1</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F124">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A125" t="s">
         <v>123</v>
       </c>
@@ -4322,8 +4822,12 @@
       <c r="E125">
         <v>2</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F125">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -4339,8 +4843,12 @@
       <c r="E126">
         <v>2</v>
       </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F126">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A127" t="s">
         <v>123</v>
       </c>
@@ -4356,8 +4864,12 @@
       <c r="E127">
         <v>2</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F127">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A128" t="s">
         <v>123</v>
       </c>
@@ -4373,8 +4885,12 @@
       <c r="E128">
         <v>1</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F128">
+        <f t="shared" ca="1" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A129" t="s">
         <v>123</v>
       </c>
@@ -4390,8 +4906,12 @@
       <c r="E129">
         <v>1</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F129">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A130" t="s">
         <v>123</v>
       </c>
@@ -4407,8 +4927,12 @@
       <c r="E130">
         <v>2</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F130">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A131" t="s">
         <v>123</v>
       </c>
@@ -4424,8 +4948,12 @@
       <c r="E131">
         <v>1</v>
       </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F131">
+        <f t="shared" ref="F131:F172" ca="1" si="2">RANDBETWEEN(0,10)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A132" t="s">
         <v>123</v>
       </c>
@@ -4441,8 +4969,12 @@
       <c r="E132">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F132">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A133" t="s">
         <v>123</v>
       </c>
@@ -4458,8 +4990,12 @@
       <c r="E133">
         <v>1</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F133">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A134" t="s">
         <v>123</v>
       </c>
@@ -4475,8 +5011,12 @@
       <c r="E134">
         <v>2</v>
       </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F134">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A135" t="s">
         <v>123</v>
       </c>
@@ -4492,8 +5032,12 @@
       <c r="E135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F135">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A136" t="s">
         <v>123</v>
       </c>
@@ -4509,8 +5053,12 @@
       <c r="E136">
         <v>2</v>
       </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F136">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A137" t="s">
         <v>123</v>
       </c>
@@ -4526,8 +5074,12 @@
       <c r="E137">
         <v>2</v>
       </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F137">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A138" t="s">
         <v>123</v>
       </c>
@@ -4543,8 +5095,12 @@
       <c r="E138">
         <v>1</v>
       </c>
-    </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F138">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A139" t="s">
         <v>123</v>
       </c>
@@ -4560,8 +5116,12 @@
       <c r="E139">
         <v>2</v>
       </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F139">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A140" t="s">
         <v>123</v>
       </c>
@@ -4577,8 +5137,12 @@
       <c r="E140">
         <v>2</v>
       </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F140">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A141" t="s">
         <v>123</v>
       </c>
@@ -4594,8 +5158,12 @@
       <c r="E141">
         <v>1</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F141">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A142" t="s">
         <v>123</v>
       </c>
@@ -4611,8 +5179,12 @@
       <c r="E142">
         <v>2</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F142">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A143" t="s">
         <v>123</v>
       </c>
@@ -4628,8 +5200,12 @@
       <c r="E143">
         <v>1</v>
       </c>
-    </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F143">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A144" t="s">
         <v>123</v>
       </c>
@@ -4645,8 +5221,12 @@
       <c r="E144">
         <v>1</v>
       </c>
-    </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F144">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A145" t="s">
         <v>123</v>
       </c>
@@ -4662,8 +5242,12 @@
       <c r="E145">
         <v>1</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F145">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A146" t="s">
         <v>123</v>
       </c>
@@ -4679,8 +5263,12 @@
       <c r="E146">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F146">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A147" t="s">
         <v>123</v>
       </c>
@@ -4696,8 +5284,12 @@
       <c r="E147">
         <v>1</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F147">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A148" t="s">
         <v>123</v>
       </c>
@@ -4713,8 +5305,12 @@
       <c r="E148">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F148">
+        <f t="shared" ca="1" si="2"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A149" t="s">
         <v>123</v>
       </c>
@@ -4730,8 +5326,12 @@
       <c r="E149">
         <v>1</v>
       </c>
-    </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F149">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A150" t="s">
         <v>123</v>
       </c>
@@ -4747,8 +5347,12 @@
       <c r="E150">
         <v>1</v>
       </c>
-    </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F150">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A151" t="s">
         <v>123</v>
       </c>
@@ -4764,8 +5368,12 @@
       <c r="E151">
         <v>1</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F151">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A152" t="s">
         <v>123</v>
       </c>
@@ -4781,8 +5389,12 @@
       <c r="E152">
         <v>1</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F152">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A153" t="s">
         <v>123</v>
       </c>
@@ -4798,8 +5410,12 @@
       <c r="E153">
         <v>1</v>
       </c>
-    </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F153">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A154" t="s">
         <v>123</v>
       </c>
@@ -4815,8 +5431,12 @@
       <c r="E154">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F154">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A155" t="s">
         <v>123</v>
       </c>
@@ -4832,8 +5452,12 @@
       <c r="E155">
         <v>1</v>
       </c>
-    </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F155">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A156" t="s">
         <v>123</v>
       </c>
@@ -4849,8 +5473,12 @@
       <c r="E156">
         <v>1</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F156">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A157" t="s">
         <v>123</v>
       </c>
@@ -4866,8 +5494,12 @@
       <c r="E157">
         <v>1</v>
       </c>
-    </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F157">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A158" t="s">
         <v>123</v>
       </c>
@@ -4883,8 +5515,12 @@
       <c r="E158">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F158">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A159" t="s">
         <v>214</v>
       </c>
@@ -4900,8 +5536,12 @@
       <c r="E159">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F159">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A160" t="s">
         <v>214</v>
       </c>
@@ -4917,8 +5557,12 @@
       <c r="E160">
         <v>1</v>
       </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F160">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A161" t="s">
         <v>214</v>
       </c>
@@ -4934,8 +5578,12 @@
       <c r="E161">
         <v>1</v>
       </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F161">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A162" t="s">
         <v>214</v>
       </c>
@@ -4951,8 +5599,12 @@
       <c r="E162">
         <v>1</v>
       </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F162">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A163" t="s">
         <v>214</v>
       </c>
@@ -4968,8 +5620,12 @@
       <c r="E163">
         <v>1</v>
       </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F163">
+        <f t="shared" ca="1" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A164" t="s">
         <v>214</v>
       </c>
@@ -4985,8 +5641,12 @@
       <c r="E164">
         <v>1</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F164">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A165" t="s">
         <v>214</v>
       </c>
@@ -5002,8 +5662,12 @@
       <c r="E165">
         <v>2</v>
       </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F165">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A166" t="s">
         <v>214</v>
       </c>
@@ -5019,8 +5683,12 @@
       <c r="E166">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F166">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A167" t="s">
         <v>214</v>
       </c>
@@ -5036,8 +5704,12 @@
       <c r="E167">
         <v>1</v>
       </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F167">
+        <f t="shared" ca="1" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A168" t="s">
         <v>214</v>
       </c>
@@ -5053,8 +5725,12 @@
       <c r="E168">
         <v>1</v>
       </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F168">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A169" t="s">
         <v>214</v>
       </c>
@@ -5070,8 +5746,12 @@
       <c r="E169">
         <v>1</v>
       </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F169">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A170" t="s">
         <v>214</v>
       </c>
@@ -5087,8 +5767,12 @@
       <c r="E170">
         <v>1</v>
       </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F170">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A171" t="s">
         <v>64</v>
       </c>
@@ -5104,8 +5788,12 @@
       <c r="E171">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="F171">
+        <f t="shared" ca="1" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A172" t="s">
         <v>64</v>
       </c>
@@ -5120,6 +5808,10 @@
       </c>
       <c r="E172">
         <v>2</v>
+      </c>
+      <c r="F172">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>